<commit_message>
calc duration in excel
</commit_message>
<xml_diff>
--- a/schedules.xlsx
+++ b/schedules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kylejow\Desktop\Mediasite-Bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8A0F23-CF45-471C-8372-3BFE8B1143F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF3D50A-B759-48EA-993F-13A4B441EA78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9030" yWindow="3030" windowWidth="28800" windowHeight="15460" xr2:uid="{7616E24A-88D1-4EA1-B65F-99333F4C0F1B}"/>
+    <workbookView xWindow="1990" yWindow="2800" windowWidth="28800" windowHeight="15460" xr2:uid="{7616E24A-88D1-4EA1-B65F-99333F4C0F1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,16 +63,16 @@
     <t>TR</t>
   </si>
   <si>
-    <t>duration_hour</t>
-  </si>
-  <si>
-    <t>duration_minute</t>
-  </si>
-  <si>
     <t>1-test_001</t>
   </si>
   <si>
     <t>1-test_002</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>duration</t>
   </si>
 </sst>
 </file>
@@ -425,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C70223B6-443F-4BB6-ABB1-EFDA9878F776}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -447,18 +447,18 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>1301</v>
@@ -469,19 +469,20 @@
       <c r="D2" s="1">
         <v>0.54166666666666663</v>
       </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="E2" s="1">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F2" t="s">
         <v>7</v>
+      </c>
+      <c r="G2" s="1">
+        <f>E2-D2</f>
+        <v>4.1666666666666741E-2</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>1303</v>
@@ -492,15 +493,28 @@
       <c r="D3" s="1">
         <v>0.64583333333333337</v>
       </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>30</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="E3" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F3" t="s">
         <v>8</v>
       </c>
+      <c r="G3" s="1">
+        <f t="shared" ref="G3:G7" si="0">E3-D3</f>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
calc duration in spreadsheet
</commit_message>
<xml_diff>
--- a/schedules.xlsx
+++ b/schedules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kylejow\Desktop\Mediasite-Bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF3D50A-B759-48EA-993F-13A4B441EA78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90480F12-6213-49B2-9301-A72406B34D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1990" yWindow="2800" windowWidth="28800" windowHeight="15460" xr2:uid="{7616E24A-88D1-4EA1-B65F-99333F4C0F1B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{7616E24A-88D1-4EA1-B65F-99333F4C0F1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>crn</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>duration</t>
+  </si>
+  <si>
+    <t>duration_hour</t>
+  </si>
+  <si>
+    <t>duration_minute</t>
   </si>
 </sst>
 </file>
@@ -425,15 +431,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C70223B6-443F-4BB6-ABB1-EFDA9878F776}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -455,8 +461,14 @@
       <c r="G1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -479,8 +491,16 @@
         <f>E2-D2</f>
         <v>4.1666666666666741E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2">
+        <f>HOUR(G2)</f>
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <f>MINUTE(G2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -500,23 +520,32 @@
         <v>8</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G7" si="0">E3-D3</f>
+        <f>E3-D3</f>
         <v>6.25E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G7" s="1"/>
+      <c r="H3">
+        <f>HOUR(G3)</f>
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <f>MINUTE(G3)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>